<commit_message>
Excel Feature: Tests fixed
Fixed some testing issues
</commit_message>
<xml_diff>
--- a/src/test/resources/visitExcelArchitectureTest.xlsx
+++ b/src/test/resources/visitExcelArchitectureTest.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Miriam\Documents\Uni\HIWI\test_version\src\test\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F963D46F-8D75-4592-A7DB-E1273BA81BD3}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ABD69583-2AC7-42D2-9891-A582750E4A15}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Activity" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="272" uniqueCount="183">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="271" uniqueCount="182">
   <si>
     <t>ID</t>
   </si>
@@ -555,9 +555,6 @@
   </si>
   <si>
     <t>beschreibung</t>
-  </si>
-  <si>
-    <t>bauteil</t>
   </si>
   <si>
     <t>kommentar</t>
@@ -1610,11 +1607,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:B54"/>
   <sheetViews>
-    <sheetView zoomScale="49" zoomScaleNormal="49" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="49" zoomScaleNormal="49" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" sqref="A1:XFD1"/>
+      <selection pane="bottomRight" activeCell="B42" sqref="B42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1627,7 +1624,7 @@
         <v>18</v>
       </c>
       <c r="B1" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
@@ -1754,7 +1751,7 @@
         <v>48</v>
       </c>
       <c r="B21" s="21" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
     </row>
     <row r="22" spans="1:2" s="22" customFormat="1" x14ac:dyDescent="0.3">
@@ -1772,7 +1769,7 @@
     </row>
     <row r="24" spans="1:2" s="24" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A24" s="24" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="25" spans="1:2" s="25" customFormat="1" x14ac:dyDescent="0.3">
@@ -1882,9 +1879,6 @@
       <c r="A42" t="s">
         <v>65</v>
       </c>
-      <c r="B42" t="s">
-        <v>176</v>
-      </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
@@ -1911,7 +1905,7 @@
         <v>70</v>
       </c>
       <c r="B47" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.3">
@@ -1919,7 +1913,7 @@
         <v>13</v>
       </c>
       <c r="B48" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.3">
@@ -1927,7 +1921,7 @@
         <v>12</v>
       </c>
       <c r="B49" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
     </row>
     <row r="50" spans="1:2" s="42" customFormat="1" x14ac:dyDescent="0.3">
@@ -3012,7 +3006,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:A14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>

</xml_diff>

<commit_message>
Excel Feature: Small bug fixes & testing
</commit_message>
<xml_diff>
--- a/src/test/resources/visitExcelArchitectureTest.xlsx
+++ b/src/test/resources/visitExcelArchitectureTest.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Miriam\Documents\Uni\HIWI\test_version\src\test\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3281CDFF-D826-4BBD-BB1F-1C88797FC7CC}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F786083C-8F07-4ABA-B5A1-C7548828D1A3}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="299" uniqueCount="198">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="297" uniqueCount="197">
   <si>
     <t>ID</t>
   </si>
@@ -603,9 +603,6 @@
   </si>
   <si>
     <t>KommentarB</t>
-  </si>
-  <si>
-    <t>Bauteil</t>
   </si>
   <si>
     <t>EigentümerPers</t>
@@ -1668,10 +1665,10 @@
   <dimension ref="A1:B54"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B25" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B26" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="B54" sqref="B54"/>
+      <selection pane="bottomRight" activeCell="B42" sqref="B42:B43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1999,24 +1996,20 @@
       <c r="A42" t="s">
         <v>65</v>
       </c>
-      <c r="B42" s="141" t="s">
-        <v>192</v>
-      </c>
+      <c r="B42" s="141"/>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
         <v>66</v>
       </c>
-      <c r="B43" s="141" t="s">
-        <v>192</v>
-      </c>
+      <c r="B43" s="141"/>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
         <v>67</v>
       </c>
       <c r="B44" s="141" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.3">
@@ -2024,7 +2017,7 @@
         <v>68</v>
       </c>
       <c r="B45" s="141" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.3">
@@ -2032,7 +2025,7 @@
         <v>69</v>
       </c>
       <c r="B46" s="141" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.3">
@@ -2069,7 +2062,7 @@
         <v>15</v>
       </c>
       <c r="B51" s="43" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
     </row>
     <row r="52" spans="1:2" s="44" customFormat="1" x14ac:dyDescent="0.3">
@@ -2085,7 +2078,7 @@
         <v>17</v>
       </c>
       <c r="B53" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
ExcelFeature: rearranged tests and added tests
added tests: testing the updated JSON for linking referred objects from the Excel files
</commit_message>
<xml_diff>
--- a/src/test/resources/visitExcelArchitectureTest.xlsx
+++ b/src/test/resources/visitExcelArchitectureTest.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Miriam\Documents\Uni\HIWI\test_version\src\test\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F786083C-8F07-4ABA-B5A1-C7548828D1A3}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC628C6E-8975-4CF7-A5EC-D93830B90DEB}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="297" uniqueCount="197">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="296" uniqueCount="197">
   <si>
     <t>ID</t>
   </si>
@@ -933,7 +933,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="142">
+  <cellXfs count="143">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -1076,6 +1076,7 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="0" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -1665,15 +1666,16 @@
   <dimension ref="A1:B54"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B26" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B13" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="B42" sqref="B42:B43"/>
+      <selection pane="bottomRight" activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="41" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
@@ -1794,8 +1796,8 @@
       <c r="A16" s="16" t="s">
         <v>43</v>
       </c>
-      <c r="B16" s="16" t="s">
-        <v>168</v>
+      <c r="B16" s="142">
+        <v>43607</v>
       </c>
     </row>
     <row r="17" spans="1:2" s="17" customFormat="1" x14ac:dyDescent="0.3">

</xml_diff>